<commit_message>
Added class CallOffFileProcessing what is inhertied from FileProcessing. It gets all methods and add one more specific for call off to remove empty rows. Thereby it is also needed to overwrite method giving complete dataframe
</commit_message>
<xml_diff>
--- a/data/output.xlsx
+++ b/data/output.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -571,6 +571,25 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>ghv</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added loop what iterates on every single row with order from call off dataframe and calls appropriate methods. First created method is to gain order as Series object and order number
</commit_message>
<xml_diff>
--- a/data/output.xlsx
+++ b/data/output.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -571,25 +571,6 @@
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>ghv</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>